<commit_message>
Change to example individual mode demo form
</commit_message>
<xml_diff>
--- a/app/config/tables/ex_ind_mode_registration_demo/forms/ex_ind_mode_registration_demo/ex_ind_mode_registration_demo.xlsx
+++ b/app/config/tables/ex_ind_mode_registration_demo/forms/ex_ind_mode_registration_demo/ex_ind_mode_registration_demo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="16230" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="16230" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="114">
   <si>
     <t>clause</t>
   </si>
@@ -76,12 +76,6 @@
     <t>assign</t>
   </si>
   <si>
-    <t>verify_user</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>begin screen</t>
   </si>
   <si>
@@ -214,42 +208,9 @@
     <t>Female</t>
   </si>
   <si>
-    <t>sites</t>
-  </si>
-  <si>
-    <t>a0</t>
-  </si>
-  <si>
-    <t>Site A</t>
-  </si>
-  <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>Site B</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>Site C</t>
-  </si>
-  <si>
-    <t>a3</t>
-  </si>
-  <si>
-    <t>Site D</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>FALSE</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -383,6 +344,42 @@
   </si>
   <si>
     <t>Custom Individual Form</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>registration_number</t>
+  </si>
+  <si>
+    <t>case_number</t>
+  </si>
+  <si>
+    <t>asylum _card</t>
+  </si>
+  <si>
+    <t>police _notes</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>disability</t>
+  </si>
+  <si>
+    <t>unaccompanied_minors</t>
+  </si>
+  <si>
+    <t>single_parent_family</t>
   </si>
 </sst>
 </file>
@@ -528,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -540,8 +537,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -921,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:D15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -978,53 +973,56 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2"/>
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B2"/>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="9" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2"/>
+      <c r="K2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="15"/>
       <c r="H3"/>
-      <c r="K3"/>
+      <c r="K3" s="1" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="17"/>
+        <v>19</v>
+      </c>
+      <c r="G4" s="15"/>
       <c r="H4"/>
       <c r="K4" s="1" t="b">
         <f>TRUE()</f>
@@ -1032,75 +1030,73 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5"/>
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B5"/>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="K5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6" s="12"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="K6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5"/>
-      <c r="K5" s="1" t="b">
+      <c r="H7"/>
+      <c r="K7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8"/>
+      <c r="K8" s="1" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6"/>
-      <c r="K6"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="K7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8" s="14"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="K8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>33</v>
@@ -1108,171 +1104,150 @@
       <c r="E9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9"/>
+      <c r="F9" s="12"/>
+      <c r="G9"/>
+      <c r="H9" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="K9" s="1" t="b">
-        <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10"/>
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B10"/>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="14"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10" s="12"/>
       <c r="G10"/>
-      <c r="H10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="H10"/>
+      <c r="K10"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
       <c r="G11"/>
       <c r="H11"/>
       <c r="K11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12"/>
+      <c r="A12"/>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="H12"/>
       <c r="K12"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13"/>
+      <c r="B13"/>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="5" t="s">
-        <v>40</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13"/>
       <c r="H13"/>
-      <c r="K13"/>
+      <c r="K13" s="1" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="F14" s="12"/>
       <c r="G14"/>
-      <c r="H14"/>
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
       <c r="K14" s="1" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15"/>
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B15"/>
-      <c r="C15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="14"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15" s="12"/>
       <c r="G15"/>
-      <c r="H15" t="s">
-        <v>28</v>
-      </c>
-      <c r="K15" s="1" t="b">
+      <c r="H15"/>
+      <c r="K15"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="H16"/>
+      <c r="K16"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17"/>
+      <c r="C17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="1" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16" s="14"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="K16"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14"/>
-      <c r="H17"/>
-      <c r="K17"/>
-    </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18"/>
-      <c r="C18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K18" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="K19"/>
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="K18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1290,64 +1265,64 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.25" style="19" customWidth="1"/>
-    <col min="2" max="2" width="23" style="20" customWidth="1"/>
+    <col min="1" max="1" width="22.25" style="17" customWidth="1"/>
+    <col min="2" max="2" width="23" style="18" customWidth="1"/>
     <col min="3" max="3" width="8.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="22" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="B2" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="B3" s="18">
+        <v>20170530</v>
+      </c>
+      <c r="C3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="B4" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
         <v>49</v>
-      </c>
-      <c r="B3" s="20">
-        <v>20170530</v>
-      </c>
-      <c r="C3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
-        <v>51</v>
       </c>
       <c r="B5"/>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>22</v>
+      <c r="A6" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1360,7 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9:B10"/>
     </sheetView>
   </sheetViews>
@@ -1375,137 +1350,137 @@
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
+        <v>51</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="25"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="25"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="23"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="25"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="23"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="25"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="25"/>
+        <v>40</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="23"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1516,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1529,191 +1504,147 @@
     <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>47</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
+        <v>36</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
+        <v>36</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
         <v>58</v>
       </c>
-      <c r="B8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>67</v>
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>69</v>
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>109</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1736,19 +1667,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="27" t="s">
+      <c r="A1" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>80</v>
+        <v>37</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1768,54 +1699,54 @@
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="27" t="s">
+      <c r="A1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="29" t="s">
-        <v>46</v>
+      <c r="E1" s="27" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>87</v>
+      <c r="A2" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>88</v>
+        <v>72</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>90</v>
+        <v>76</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1843,32 +1774,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>99</v>
+      <c r="A1" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1891,68 +1822,68 @@
     <col min="2" max="2" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="28" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>15</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1976,35 +1907,35 @@
     <col min="4" max="4" width="24.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-    </row>
-    <row r="3" spans="1:4" ht="236.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28" t="s">
-        <v>112</v>
+      <c r="C1" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+    </row>
+    <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change name of individual demo form to be more user friendly
</commit_message>
<xml_diff>
--- a/app/config/tables/ex_ind_mode_registration_demo/forms/ex_ind_mode_registration_demo/ex_ind_mode_registration_demo.xlsx
+++ b/app/config/tables/ex_ind_mode_registration_demo/forms/ex_ind_mode_registration_demo/ex_ind_mode_registration_demo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="16230" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="16230" tabRatio="989" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -343,9 +343,6 @@
     <t>ex_ind_mode_registration_demo</t>
   </si>
   <si>
-    <t>Custom Individual Form</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
@@ -380,6 +377,9 @@
   </si>
   <si>
     <t>single_parent_family</t>
+  </si>
+  <si>
+    <t>Individual</t>
   </si>
 </sst>
 </file>
@@ -918,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D15" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -1259,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="B5"/>
       <c r="C5" s="1" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1520,7 +1520,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
         <v>54</v>
@@ -1531,7 +1531,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
         <v>55</v>
@@ -1542,7 +1542,7 @@
         <v>36</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
@@ -1553,7 +1553,7 @@
         <v>36</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
         <v>57</v>
@@ -1564,7 +1564,7 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
         <v>58</v>
@@ -1575,7 +1575,7 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
         <v>59</v>
@@ -1586,7 +1586,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
         <v>60</v>
@@ -1597,7 +1597,7 @@
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" t="s">
         <v>61</v>
@@ -1608,7 +1608,7 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" t="s">
         <v>62</v>
@@ -1619,7 +1619,7 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s">
         <v>63</v>
@@ -1630,7 +1630,7 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" t="s">
         <v>64</v>
@@ -1641,7 +1641,7 @@
         <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
         <v>65</v>

</xml_diff>